<commit_message>
ATLAS fact sheeet, events and info update, and ATLAS Data 4.5.1: mitigations updates, STIX with ATT&CK v14.1
</commit_message>
<xml_diff>
--- a/static/excel-files/atlas-tactics.xlsx
+++ b/static/excel-files/atlas-tactics.xlsx
@@ -79,46 +79,46 @@
     <t>AML.TA0003</t>
   </si>
   <si>
-    <t>x-mitre-tactic--169cdf3d-886b-4d3e-a26d-11a848920ea8</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--da8d1d9d-c45d-4d56-8874-d7cd5886dc25</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--e67a0f3d-a541-401f-801e-e62a9fdeca70</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--e81ccab1-e5f8-4d4f-be66-24dbe74fe5db</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--95274328-9e38-4bdd-9d2e-0e80e1256ff0</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--02d1fc74-a19e-406f-9ecc-df96a8d18856</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--7b38d743-e6b2-4a99-a497-bbc97db9a761</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--57175629-3f53-4980-a99d-8725df069f91</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--cf90e8f7-7829-431f-866f-66e6dd9e18a2</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--d4010b82-406a-46ba-83a1-23c16db77604</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--714edce4-f9ef-4b9a-b0ae-56e70a3cb15c</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--4acc5de3-5a7c-4ac8-8e7f-0e9f25e7e725</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--c79e43f1-2a18-48d4-af61-40091b1f1a37</t>
-  </si>
-  <si>
-    <t>x-mitre-tactic--90786da6-b4a6-4741-9bab-a87fdf42a05b</t>
+    <t>x-mitre-tactic--afe18db5-cd3b-404c-8993-3aaf488c5f62</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--f3deea7c-6d5a-49e7-ae3a-d70afc7889c9</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--9633dd67-f5e8-4a19-88aa-c9b6fcf9596c</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--c8c04179-cc2c-4a1d-b392-e6d4c42c3493</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--d9deeb4d-c193-469d-a1c8-52e6d145da0c</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--2538ccce-34dd-4470-8c3f-747be088b4e6</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--f7d86c97-d8a6-4b81-a4a3-b49191faeced</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--876860aa-e340-435c-824b-b5dd011c4c95</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--c05767a2-5965-4618-b66e-6a7fffed256a</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--813efb61-5bed-439d-a264-1b4e0ab89c37</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--8bb9a040-d075-4566-966d-4a6a588f4fad</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--39d150db-6130-4b2e-81e5-754b344a6a00</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--d4d10ed9-f6d7-4774-a9f0-68bf4970c5bd</t>
+  </si>
+  <si>
+    <t>x-mitre-tactic--4cd8009a-c196-4c3d-8eae-87afa661ed8e</t>
   </si>
   <si>
     <t>Collection</t>
@@ -307,7 +307,7 @@
     <t>https://atlas.mitre.org/tactics/AML.TA0003</t>
   </si>
   <si>
-    <t>31 October 2023</t>
+    <t>12 January 2024</t>
   </si>
 </sst>
 </file>

</xml_diff>